<commit_message>
fix = benerin file path
</commit_message>
<xml_diff>
--- a/Persediaan1.xlsx
+++ b/Persediaan1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah Bila\SMT 2\Prokom\prokom ori\Kelompok-1-sistem-pembelian-sepatu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F8BFA5-4B19-4E49-B270-654AE8522FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA0A8EF-9F02-4123-9752-F8DCB37B7860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="26">
   <si>
     <t>jenis</t>
   </si>
@@ -158,10 +158,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="91" workbookViewId="0">
+      <selection activeCell="J92" sqref="J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,19 +511,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1">
         <v>37</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>11111111</v>
       </c>
       <c r="F2">
@@ -534,13 +534,19 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D3" s="1">
         <v>38</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>11111112</v>
       </c>
       <c r="F3">
@@ -551,13 +557,19 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D4" s="1">
         <v>39</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>11111113</v>
       </c>
       <c r="F4">
@@ -568,13 +580,19 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D5" s="1">
         <v>40</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>11111114</v>
       </c>
       <c r="F5">
@@ -585,13 +603,19 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" s="1">
         <v>41</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>11111115</v>
       </c>
       <c r="F6">
@@ -602,13 +626,19 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D7" s="1">
         <v>42</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>11111116</v>
       </c>
       <c r="F7">
@@ -619,13 +649,19 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="1">
         <v>43</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>11111117</v>
       </c>
       <c r="F8">
@@ -636,13 +672,19 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D9" s="1">
         <v>44</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>11111118</v>
       </c>
       <c r="F9">
@@ -653,13 +695,19 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D10" s="1">
         <v>45</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>11111119</v>
       </c>
       <c r="F10">
@@ -670,17 +718,19 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="1">
         <v>37</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>11111120</v>
       </c>
       <c r="F11">
@@ -691,13 +741,19 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D12" s="1">
         <v>38</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>11111121</v>
       </c>
       <c r="F12">
@@ -708,13 +764,19 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D13" s="1">
         <v>39</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>11111122</v>
       </c>
       <c r="F13">
@@ -725,13 +787,19 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D14" s="1">
         <v>40</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>11111123</v>
       </c>
       <c r="F14">
@@ -742,13 +810,19 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D15" s="1">
         <v>41</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>11111124</v>
       </c>
       <c r="F15">
@@ -759,13 +833,19 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D16" s="1">
         <v>42</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>11111125</v>
       </c>
       <c r="F16">
@@ -776,13 +856,19 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D17" s="1">
         <v>43</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>11111126</v>
       </c>
       <c r="F17">
@@ -793,13 +879,19 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D18" s="1">
         <v>44</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>11111127</v>
       </c>
       <c r="F18">
@@ -810,13 +902,19 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D19" s="1">
         <v>45</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>11111128</v>
       </c>
       <c r="F19">
@@ -827,17 +925,19 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="1">
         <v>37</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>11111129</v>
       </c>
       <c r="F20">
@@ -848,13 +948,19 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D21" s="1">
         <v>38</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>11111130</v>
       </c>
       <c r="F21">
@@ -865,13 +971,19 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D22" s="1">
         <v>39</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>11111131</v>
       </c>
       <c r="F22">
@@ -882,13 +994,19 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D23" s="1">
         <v>40</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>11111132</v>
       </c>
       <c r="F23">
@@ -899,13 +1017,19 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D24" s="1">
         <v>41</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>11111133</v>
       </c>
       <c r="F24">
@@ -916,13 +1040,19 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D25" s="1">
         <v>42</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>11111134</v>
       </c>
       <c r="F25">
@@ -933,13 +1063,19 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D26" s="1">
         <v>43</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>11111135</v>
       </c>
       <c r="F26">
@@ -950,13 +1086,19 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D27" s="1">
         <v>44</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>11111136</v>
       </c>
       <c r="F27">
@@ -967,13 +1109,19 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D28" s="1">
         <v>45</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>11111137</v>
       </c>
       <c r="F28">
@@ -984,17 +1132,19 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2" t="s">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="1">
         <v>37</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>11111138</v>
       </c>
       <c r="F29">
@@ -1005,13 +1155,19 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D30" s="1">
         <v>38</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>11111139</v>
       </c>
       <c r="F30">
@@ -1022,13 +1178,19 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D31" s="1">
         <v>39</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>11111140</v>
       </c>
       <c r="F31">
@@ -1039,13 +1201,19 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D32" s="1">
         <v>40</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>11111141</v>
       </c>
       <c r="F32">
@@ -1056,13 +1224,19 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D33" s="1">
         <v>41</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>11111142</v>
       </c>
       <c r="F33">
@@ -1073,13 +1247,19 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D34" s="1">
         <v>42</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>11111143</v>
       </c>
       <c r="F34">
@@ -1090,13 +1270,19 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D35" s="1">
         <v>43</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>11111144</v>
       </c>
       <c r="F35">
@@ -1107,13 +1293,19 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="A36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D36" s="1">
         <v>44</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>11111145</v>
       </c>
       <c r="F36">
@@ -1124,13 +1316,19 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D37" s="1">
         <v>45</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>11111146</v>
       </c>
       <c r="F37">
@@ -1141,19 +1339,19 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="A38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="3">
         <v>550</v>
       </c>
       <c r="D38" s="1">
         <v>37</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>11111147</v>
       </c>
       <c r="F38">
@@ -1164,13 +1362,19 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="3">
+        <v>550</v>
+      </c>
       <c r="D39" s="1">
         <v>38</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>11111148</v>
       </c>
       <c r="F39">
@@ -1181,13 +1385,19 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="A40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="3">
+        <v>550</v>
+      </c>
       <c r="D40" s="1">
         <v>39</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>11111149</v>
       </c>
       <c r="F40">
@@ -1198,13 +1408,19 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="A41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="3">
+        <v>550</v>
+      </c>
       <c r="D41" s="1">
         <v>40</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>11111150</v>
       </c>
       <c r="F41">
@@ -1215,13 +1431,19 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="A42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="3">
+        <v>550</v>
+      </c>
       <c r="D42" s="1">
         <v>41</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>11111151</v>
       </c>
       <c r="F42">
@@ -1232,13 +1454,19 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="A43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="3">
+        <v>550</v>
+      </c>
       <c r="D43" s="1">
         <v>42</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>11111152</v>
       </c>
       <c r="F43">
@@ -1249,13 +1477,19 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="3">
+        <v>550</v>
+      </c>
       <c r="D44" s="1">
         <v>43</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>11111153</v>
       </c>
       <c r="F44">
@@ -1266,13 +1500,19 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="3">
+        <v>550</v>
+      </c>
       <c r="D45" s="1">
         <v>44</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>11111154</v>
       </c>
       <c r="F45">
@@ -1283,13 +1523,19 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="A46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="3">
+        <v>550</v>
+      </c>
       <c r="D46" s="1">
         <v>45</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>11111155</v>
       </c>
       <c r="F46">
@@ -1300,17 +1546,19 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2" t="s">
+      <c r="A47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D47" s="1">
         <v>37</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <v>11111156</v>
       </c>
       <c r="F47">
@@ -1321,13 +1569,19 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="A48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D48" s="1">
         <v>38</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>11111157</v>
       </c>
       <c r="F48">
@@ -1338,13 +1592,19 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="A49" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D49" s="1">
         <v>39</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>11111158</v>
       </c>
       <c r="F49">
@@ -1355,13 +1615,19 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="A50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D50" s="1">
         <v>40</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>11111159</v>
       </c>
       <c r="F50">
@@ -1372,13 +1638,19 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="A51" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D51" s="1">
         <v>41</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="2">
         <v>11111160</v>
       </c>
       <c r="F51">
@@ -1389,13 +1661,19 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="A52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D52" s="1">
         <v>42</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="2">
         <v>11111161</v>
       </c>
       <c r="F52">
@@ -1406,13 +1684,19 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="A53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D53" s="1">
         <v>43</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="2">
         <v>11111162</v>
       </c>
       <c r="F53">
@@ -1423,13 +1707,19 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="A54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D54" s="1">
         <v>44</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="2">
         <v>11111163</v>
       </c>
       <c r="F54">
@@ -1440,13 +1730,19 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="A55" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D55" s="1">
         <v>45</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="2">
         <v>11111164</v>
       </c>
       <c r="F55">
@@ -1457,17 +1753,19 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="A56" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D56" s="1">
         <v>37</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="2">
         <v>11111165</v>
       </c>
       <c r="F56">
@@ -1478,13 +1776,19 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="A57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D57" s="1">
         <v>38</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="2">
         <v>11111166</v>
       </c>
       <c r="F57">
@@ -1495,13 +1799,19 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="A58" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D58" s="1">
         <v>39</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="2">
         <v>11111167</v>
       </c>
       <c r="F58">
@@ -1512,13 +1822,19 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="A59" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D59" s="1">
         <v>40</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="2">
         <v>11111168</v>
       </c>
       <c r="F59">
@@ -1529,13 +1845,19 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="A60" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D60" s="1">
         <v>41</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="2">
         <v>11111169</v>
       </c>
       <c r="F60">
@@ -1546,13 +1868,19 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="A61" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D61" s="1">
         <v>42</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="2">
         <v>11111170</v>
       </c>
       <c r="F61">
@@ -1563,13 +1891,19 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="A62" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D62" s="1">
         <v>43</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E62" s="2">
         <v>11111171</v>
       </c>
       <c r="F62">
@@ -1580,13 +1914,19 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="A63" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D63" s="1">
         <v>44</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63" s="2">
         <v>11111172</v>
       </c>
       <c r="F63">
@@ -1597,13 +1937,19 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="A64" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D64" s="1">
         <v>45</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64" s="2">
         <v>11111173</v>
       </c>
       <c r="F64">
@@ -1614,15 +1960,19 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2" t="s">
+      <c r="A65" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D65" s="1">
         <v>37</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65" s="2">
         <v>11111174</v>
       </c>
       <c r="F65">
@@ -1633,13 +1983,19 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="A66" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D66" s="1">
         <v>38</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="2">
         <v>11111175</v>
       </c>
       <c r="F66">
@@ -1650,13 +2006,19 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
+      <c r="A67" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D67" s="1">
         <v>39</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E67" s="2">
         <v>11111176</v>
       </c>
       <c r="F67">
@@ -1667,13 +2029,19 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="A68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D68" s="1">
         <v>40</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E68" s="2">
         <v>11111177</v>
       </c>
       <c r="F68">
@@ -1684,13 +2052,19 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="A69" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D69" s="1">
         <v>41</v>
       </c>
-      <c r="E69" s="3">
+      <c r="E69" s="2">
         <v>11111178</v>
       </c>
       <c r="F69">
@@ -1701,13 +2075,19 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="A70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D70" s="1">
         <v>42</v>
       </c>
-      <c r="E70" s="3">
+      <c r="E70" s="2">
         <v>11111179</v>
       </c>
       <c r="F70">
@@ -1718,13 +2098,19 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="A71" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D71" s="1">
         <v>43</v>
       </c>
-      <c r="E71" s="3">
+      <c r="E71" s="2">
         <v>11111180</v>
       </c>
       <c r="F71">
@@ -1735,13 +2121,19 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
+      <c r="A72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D72" s="1">
         <v>44</v>
       </c>
-      <c r="E72" s="3">
+      <c r="E72" s="2">
         <v>11111181</v>
       </c>
       <c r="F72">
@@ -1752,13 +2144,19 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
+      <c r="A73" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D73" s="1">
         <v>45</v>
       </c>
-      <c r="E73" s="3">
+      <c r="E73" s="2">
         <v>11111182</v>
       </c>
       <c r="F73">
@@ -1769,19 +2167,19 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C74" s="2" t="s">
+      <c r="B74" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D74" s="1">
         <v>37</v>
       </c>
-      <c r="E74" s="3">
+      <c r="E74" s="2">
         <v>11111183</v>
       </c>
       <c r="F74">
@@ -1792,13 +2190,19 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
+      <c r="A75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D75" s="1">
         <v>38</v>
       </c>
-      <c r="E75" s="3">
+      <c r="E75" s="2">
         <v>11111184</v>
       </c>
       <c r="F75">
@@ -1809,13 +2213,19 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
+      <c r="A76" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D76" s="1">
         <v>39</v>
       </c>
-      <c r="E76" s="3">
+      <c r="E76" s="2">
         <v>11111185</v>
       </c>
       <c r="F76">
@@ -1826,13 +2236,19 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
+      <c r="A77" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D77" s="1">
         <v>40</v>
       </c>
-      <c r="E77" s="3">
+      <c r="E77" s="2">
         <v>11111186</v>
       </c>
       <c r="F77">
@@ -1843,13 +2259,19 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
+      <c r="A78" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D78" s="1">
         <v>41</v>
       </c>
-      <c r="E78" s="3">
+      <c r="E78" s="2">
         <v>11111187</v>
       </c>
       <c r="F78">
@@ -1860,13 +2282,19 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
+      <c r="A79" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D79" s="1">
         <v>42</v>
       </c>
-      <c r="E79" s="3">
+      <c r="E79" s="2">
         <v>11111188</v>
       </c>
       <c r="F79">
@@ -1877,13 +2305,19 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
+      <c r="A80" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D80" s="1">
         <v>43</v>
       </c>
-      <c r="E80" s="3">
+      <c r="E80" s="2">
         <v>11111189</v>
       </c>
       <c r="F80">
@@ -1894,13 +2328,19 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
+      <c r="A81" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D81" s="1">
         <v>44</v>
       </c>
-      <c r="E81" s="3">
+      <c r="E81" s="2">
         <v>11111190</v>
       </c>
       <c r="F81">
@@ -1911,13 +2351,19 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
+      <c r="A82" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D82" s="1">
         <v>45</v>
       </c>
-      <c r="E82" s="3">
+      <c r="E82" s="2">
         <v>11111191</v>
       </c>
       <c r="F82">
@@ -1928,17 +2374,19 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2" t="s">
+      <c r="A83" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D83" s="1">
         <v>37</v>
       </c>
-      <c r="E83" s="3">
+      <c r="E83" s="2">
         <v>11111192</v>
       </c>
       <c r="F83">
@@ -1949,13 +2397,19 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
+      <c r="A84" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D84" s="1">
         <v>38</v>
       </c>
-      <c r="E84" s="3">
+      <c r="E84" s="2">
         <v>11111193</v>
       </c>
       <c r="F84">
@@ -1966,13 +2420,19 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
+      <c r="A85" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D85" s="1">
         <v>39</v>
       </c>
-      <c r="E85" s="3">
+      <c r="E85" s="2">
         <v>11111194</v>
       </c>
       <c r="F85">
@@ -1983,13 +2443,19 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
+      <c r="A86" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D86" s="1">
         <v>40</v>
       </c>
-      <c r="E86" s="3">
+      <c r="E86" s="2">
         <v>11111195</v>
       </c>
       <c r="F86">
@@ -2000,13 +2466,19 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
+      <c r="A87" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D87" s="1">
         <v>41</v>
       </c>
-      <c r="E87" s="3">
+      <c r="E87" s="2">
         <v>11111196</v>
       </c>
       <c r="F87">
@@ -2017,13 +2489,19 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
+      <c r="A88" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D88" s="1">
         <v>42</v>
       </c>
-      <c r="E88" s="3">
+      <c r="E88" s="2">
         <v>11111197</v>
       </c>
       <c r="F88">
@@ -2034,13 +2512,19 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
+      <c r="A89" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D89" s="1">
         <v>43</v>
       </c>
-      <c r="E89" s="3">
+      <c r="E89" s="2">
         <v>11111198</v>
       </c>
       <c r="F89">
@@ -2051,13 +2535,19 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
+      <c r="A90" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D90" s="1">
         <v>44</v>
       </c>
-      <c r="E90" s="3">
+      <c r="E90" s="2">
         <v>11111199</v>
       </c>
       <c r="F90">
@@ -2068,13 +2558,19 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
+      <c r="A91" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D91" s="1">
         <v>45</v>
       </c>
-      <c r="E91" s="3">
+      <c r="E91" s="2">
         <v>11111200</v>
       </c>
       <c r="F91">
@@ -2085,30 +2581,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="B56:B73"/>
-    <mergeCell ref="B47:B55"/>
-    <mergeCell ref="C20:C28"/>
-    <mergeCell ref="C29:C37"/>
-    <mergeCell ref="B11:B19"/>
-    <mergeCell ref="A74:A91"/>
-    <mergeCell ref="A2:A37"/>
-    <mergeCell ref="C65:C73"/>
-    <mergeCell ref="C47:C55"/>
-    <mergeCell ref="A38:A73"/>
-    <mergeCell ref="C56:C64"/>
-    <mergeCell ref="B29:B37"/>
-    <mergeCell ref="B38:B46"/>
-    <mergeCell ref="C11:C19"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="B83:B91"/>
-    <mergeCell ref="B74:B82"/>
-    <mergeCell ref="C38:C46"/>
-    <mergeCell ref="B20:B28"/>
-    <mergeCell ref="C74:C82"/>
-    <mergeCell ref="C83:C91"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix = bikin def kasir main menu
</commit_message>
<xml_diff>
--- a/Persediaan1.xlsx
+++ b/Persediaan1.xlsx
@@ -484,7 +484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,51 +532,41 @@
     <row r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
+        <v>37</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11111183</v>
+      </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>750000</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>Flip Flops</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
-      </c>
+      <c r="A3" s="4" t="n"/>
+      <c r="B3" s="4" t="n"/>
+      <c r="C3" s="4" t="n"/>
       <c r="D3" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E3" t="n">
-        <v>11111183</v>
+        <v>11111184</v>
       </c>
       <c r="F3" t="n">
         <v>750000</v>
@@ -590,10 +580,10 @@
       <c r="B4" s="4" t="n"/>
       <c r="C4" s="4" t="n"/>
       <c r="D4" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E4" t="n">
-        <v>11111184</v>
+        <v>11111185</v>
       </c>
       <c r="F4" t="n">
         <v>750000</v>
@@ -607,10 +597,10 @@
       <c r="B5" s="4" t="n"/>
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" t="n">
-        <v>11111185</v>
+        <v>11111186</v>
       </c>
       <c r="F5" t="n">
         <v>750000</v>
@@ -624,10 +614,10 @@
       <c r="B6" s="4" t="n"/>
       <c r="C6" s="4" t="n"/>
       <c r="D6" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" t="n">
-        <v>11111186</v>
+        <v>11111187</v>
       </c>
       <c r="F6" t="n">
         <v>750000</v>
@@ -641,10 +631,10 @@
       <c r="B7" s="4" t="n"/>
       <c r="C7" s="4" t="n"/>
       <c r="D7" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E7" t="n">
-        <v>11111187</v>
+        <v>11111188</v>
       </c>
       <c r="F7" t="n">
         <v>750000</v>
@@ -658,10 +648,10 @@
       <c r="B8" s="4" t="n"/>
       <c r="C8" s="4" t="n"/>
       <c r="D8" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" t="n">
-        <v>11111188</v>
+        <v>11111189</v>
       </c>
       <c r="F8" t="n">
         <v>750000</v>
@@ -675,10 +665,10 @@
       <c r="B9" s="4" t="n"/>
       <c r="C9" s="4" t="n"/>
       <c r="D9" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" t="n">
-        <v>11111189</v>
+        <v>11111190</v>
       </c>
       <c r="F9" t="n">
         <v>750000</v>
@@ -692,10 +682,10 @@
       <c r="B10" s="4" t="n"/>
       <c r="C10" s="4" t="n"/>
       <c r="D10" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E10" t="n">
-        <v>11111190</v>
+        <v>11111191</v>
       </c>
       <c r="F10" t="n">
         <v>750000</v>
@@ -706,16 +696,24 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="n"/>
-      <c r="B11" s="4" t="n"/>
-      <c r="C11" s="4" t="n"/>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nike </t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Benassi </t>
+        </is>
+      </c>
       <c r="D11" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E11" t="n">
-        <v>11111191</v>
+        <v>11111192</v>
       </c>
       <c r="F11" t="n">
-        <v>750000</v>
+        <v>500000</v>
       </c>
       <c r="G11" t="n">
         <v>10</v>
@@ -723,21 +721,13 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="n"/>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Nike </t>
-        </is>
-      </c>
-      <c r="C12" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Benassi </t>
-        </is>
-      </c>
+      <c r="B12" s="4" t="n"/>
+      <c r="C12" s="4" t="n"/>
       <c r="D12" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" t="n">
-        <v>11111192</v>
+        <v>11111193</v>
       </c>
       <c r="F12" t="n">
         <v>500000</v>
@@ -751,10 +741,10 @@
       <c r="B13" s="4" t="n"/>
       <c r="C13" s="4" t="n"/>
       <c r="D13" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" t="n">
-        <v>11111193</v>
+        <v>11111194</v>
       </c>
       <c r="F13" t="n">
         <v>500000</v>
@@ -768,10 +758,10 @@
       <c r="B14" s="4" t="n"/>
       <c r="C14" s="4" t="n"/>
       <c r="D14" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E14" t="n">
-        <v>11111194</v>
+        <v>11111195</v>
       </c>
       <c r="F14" t="n">
         <v>500000</v>
@@ -785,10 +775,10 @@
       <c r="B15" s="4" t="n"/>
       <c r="C15" s="4" t="n"/>
       <c r="D15" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" t="n">
-        <v>11111195</v>
+        <v>11111196</v>
       </c>
       <c r="F15" t="n">
         <v>500000</v>
@@ -802,10 +792,10 @@
       <c r="B16" s="4" t="n"/>
       <c r="C16" s="4" t="n"/>
       <c r="D16" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E16" t="n">
-        <v>11111196</v>
+        <v>11111197</v>
       </c>
       <c r="F16" t="n">
         <v>500000</v>
@@ -819,10 +809,10 @@
       <c r="B17" s="4" t="n"/>
       <c r="C17" s="4" t="n"/>
       <c r="D17" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" t="n">
-        <v>11111197</v>
+        <v>11111198</v>
       </c>
       <c r="F17" t="n">
         <v>500000</v>
@@ -836,10 +826,10 @@
       <c r="B18" s="4" t="n"/>
       <c r="C18" s="4" t="n"/>
       <c r="D18" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" t="n">
-        <v>11111198</v>
+        <v>11111199</v>
       </c>
       <c r="F18" t="n">
         <v>500000</v>
@@ -853,10 +843,10 @@
       <c r="B19" s="4" t="n"/>
       <c r="C19" s="4" t="n"/>
       <c r="D19" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E19" t="n">
-        <v>11111199</v>
+        <v>11111200</v>
       </c>
       <c r="F19" t="n">
         <v>500000</v>
@@ -866,43 +856,43 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="n"/>
-      <c r="B20" s="4" t="n"/>
-      <c r="C20" s="4" t="n"/>
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>Adidas</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>Adizero</t>
+        </is>
+      </c>
       <c r="D20" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E20" t="n">
-        <v>11111200</v>
+        <v>11111138</v>
       </c>
       <c r="F20" t="n">
-        <v>500000</v>
+        <v>3000000</v>
       </c>
       <c r="G20" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="inlineStr">
-        <is>
-          <t>Running</t>
-        </is>
-      </c>
-      <c r="B21" s="4" t="inlineStr">
-        <is>
-          <t>Adidas</t>
-        </is>
-      </c>
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>Adizero</t>
-        </is>
-      </c>
+      <c r="A21" s="4" t="n"/>
+      <c r="B21" s="4" t="n"/>
+      <c r="C21" s="4" t="n"/>
       <c r="D21" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21" t="n">
-        <v>11111138</v>
+        <v>11111139</v>
       </c>
       <c r="F21" t="n">
         <v>3000000</v>
@@ -916,10 +906,10 @@
       <c r="B22" s="4" t="n"/>
       <c r="C22" s="4" t="n"/>
       <c r="D22" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E22" t="n">
-        <v>11111139</v>
+        <v>11111140</v>
       </c>
       <c r="F22" t="n">
         <v>3000000</v>
@@ -933,10 +923,10 @@
       <c r="B23" s="4" t="n"/>
       <c r="C23" s="4" t="n"/>
       <c r="D23" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E23" t="n">
-        <v>11111140</v>
+        <v>11111141</v>
       </c>
       <c r="F23" t="n">
         <v>3000000</v>
@@ -950,10 +940,10 @@
       <c r="B24" s="4" t="n"/>
       <c r="C24" s="4" t="n"/>
       <c r="D24" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24" t="n">
-        <v>11111141</v>
+        <v>11111142</v>
       </c>
       <c r="F24" t="n">
         <v>3000000</v>
@@ -967,10 +957,10 @@
       <c r="B25" s="4" t="n"/>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E25" t="n">
-        <v>11111142</v>
+        <v>11111143</v>
       </c>
       <c r="F25" t="n">
         <v>3000000</v>
@@ -984,10 +974,10 @@
       <c r="B26" s="4" t="n"/>
       <c r="C26" s="4" t="n"/>
       <c r="D26" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E26" t="n">
-        <v>11111143</v>
+        <v>11111144</v>
       </c>
       <c r="F26" t="n">
         <v>3000000</v>
@@ -1001,10 +991,10 @@
       <c r="B27" s="4" t="n"/>
       <c r="C27" s="4" t="n"/>
       <c r="D27" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E27" t="n">
-        <v>11111144</v>
+        <v>11111145</v>
       </c>
       <c r="F27" t="n">
         <v>3000000</v>
@@ -1018,10 +1008,10 @@
       <c r="B28" s="4" t="n"/>
       <c r="C28" s="4" t="n"/>
       <c r="D28" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E28" t="n">
-        <v>11111145</v>
+        <v>11111146</v>
       </c>
       <c r="F28" t="n">
         <v>3000000</v>
@@ -1032,16 +1022,24 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="n"/>
-      <c r="B29" s="4" t="n"/>
-      <c r="C29" s="4" t="n"/>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>Asics</t>
+        </is>
+      </c>
+      <c r="C29" s="4" t="inlineStr">
+        <is>
+          <t>Gel-Nimbus</t>
+        </is>
+      </c>
       <c r="D29" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E29" t="n">
-        <v>11111146</v>
+        <v>11111120</v>
       </c>
       <c r="F29" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G29" t="n">
         <v>10</v>
@@ -1049,21 +1047,13 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="n"/>
-      <c r="B30" s="4" t="inlineStr">
-        <is>
-          <t>Asics</t>
-        </is>
-      </c>
-      <c r="C30" s="4" t="inlineStr">
-        <is>
-          <t>Gel-Nimbus</t>
-        </is>
-      </c>
+      <c r="B30" s="4" t="n"/>
+      <c r="C30" s="4" t="n"/>
       <c r="D30" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E30" t="n">
-        <v>11111120</v>
+        <v>11111121</v>
       </c>
       <c r="F30" t="n">
         <v>4000000</v>
@@ -1077,10 +1067,10 @@
       <c r="B31" s="4" t="n"/>
       <c r="C31" s="4" t="n"/>
       <c r="D31" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E31" t="n">
-        <v>11111121</v>
+        <v>11111122</v>
       </c>
       <c r="F31" t="n">
         <v>4000000</v>
@@ -1094,10 +1084,10 @@
       <c r="B32" s="4" t="n"/>
       <c r="C32" s="4" t="n"/>
       <c r="D32" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E32" t="n">
-        <v>11111122</v>
+        <v>11111123</v>
       </c>
       <c r="F32" t="n">
         <v>4000000</v>
@@ -1111,10 +1101,10 @@
       <c r="B33" s="4" t="n"/>
       <c r="C33" s="4" t="n"/>
       <c r="D33" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E33" t="n">
-        <v>11111123</v>
+        <v>11111124</v>
       </c>
       <c r="F33" t="n">
         <v>4000000</v>
@@ -1128,10 +1118,10 @@
       <c r="B34" s="4" t="n"/>
       <c r="C34" s="4" t="n"/>
       <c r="D34" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E34" t="n">
-        <v>11111124</v>
+        <v>11111125</v>
       </c>
       <c r="F34" t="n">
         <v>4000000</v>
@@ -1145,10 +1135,10 @@
       <c r="B35" s="4" t="n"/>
       <c r="C35" s="4" t="n"/>
       <c r="D35" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E35" t="n">
-        <v>11111125</v>
+        <v>11111126</v>
       </c>
       <c r="F35" t="n">
         <v>4000000</v>
@@ -1162,10 +1152,10 @@
       <c r="B36" s="4" t="n"/>
       <c r="C36" s="4" t="n"/>
       <c r="D36" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E36" t="n">
-        <v>11111126</v>
+        <v>11111127</v>
       </c>
       <c r="F36" t="n">
         <v>4000000</v>
@@ -1179,10 +1169,10 @@
       <c r="B37" s="4" t="n"/>
       <c r="C37" s="4" t="n"/>
       <c r="D37" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E37" t="n">
-        <v>11111127</v>
+        <v>11111128</v>
       </c>
       <c r="F37" t="n">
         <v>4000000</v>
@@ -1193,44 +1183,44 @@
     </row>
     <row r="38">
       <c r="A38" s="4" t="n"/>
-      <c r="B38" s="4" t="n"/>
-      <c r="C38" s="4" t="n"/>
+      <c r="B38" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C38" s="4" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
+      </c>
       <c r="D38" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E38" t="n">
-        <v>11111128</v>
+        <v>11111111</v>
       </c>
       <c r="F38" t="n">
-        <v>4000000</v>
+        <v>2000000</v>
       </c>
       <c r="G38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="n"/>
-      <c r="B39" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hoka </t>
-        </is>
-      </c>
-      <c r="C39" s="4" t="inlineStr">
-        <is>
-          <t>Arahi 7</t>
-        </is>
-      </c>
+      <c r="B39" s="4" t="n"/>
+      <c r="C39" s="4" t="n"/>
       <c r="D39" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E39" t="n">
-        <v>11111111</v>
+        <v>11111112</v>
       </c>
       <c r="F39" t="n">
         <v>2000000</v>
       </c>
       <c r="G39" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
@@ -1238,10 +1228,10 @@
       <c r="B40" s="4" t="n"/>
       <c r="C40" s="4" t="n"/>
       <c r="D40" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E40" t="n">
-        <v>11111112</v>
+        <v>11111113</v>
       </c>
       <c r="F40" t="n">
         <v>2000000</v>
@@ -1255,10 +1245,10 @@
       <c r="B41" s="4" t="n"/>
       <c r="C41" s="4" t="n"/>
       <c r="D41" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E41" t="n">
-        <v>11111113</v>
+        <v>11111114</v>
       </c>
       <c r="F41" t="n">
         <v>2000000</v>
@@ -1272,10 +1262,10 @@
       <c r="B42" s="4" t="n"/>
       <c r="C42" s="4" t="n"/>
       <c r="D42" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E42" t="n">
-        <v>11111114</v>
+        <v>11111115</v>
       </c>
       <c r="F42" t="n">
         <v>2000000</v>
@@ -1289,10 +1279,10 @@
       <c r="B43" s="4" t="n"/>
       <c r="C43" s="4" t="n"/>
       <c r="D43" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E43" t="n">
-        <v>11111115</v>
+        <v>11111116</v>
       </c>
       <c r="F43" t="n">
         <v>2000000</v>
@@ -1306,10 +1296,10 @@
       <c r="B44" s="4" t="n"/>
       <c r="C44" s="4" t="n"/>
       <c r="D44" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E44" t="n">
-        <v>11111116</v>
+        <v>11111117</v>
       </c>
       <c r="F44" t="n">
         <v>2000000</v>
@@ -1323,10 +1313,10 @@
       <c r="B45" s="4" t="n"/>
       <c r="C45" s="4" t="n"/>
       <c r="D45" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E45" t="n">
-        <v>11111117</v>
+        <v>11111118</v>
       </c>
       <c r="F45" t="n">
         <v>2000000</v>
@@ -1340,10 +1330,10 @@
       <c r="B46" s="4" t="n"/>
       <c r="C46" s="4" t="n"/>
       <c r="D46" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E46" t="n">
-        <v>11111118</v>
+        <v>11111119</v>
       </c>
       <c r="F46" t="n">
         <v>2000000</v>
@@ -1354,16 +1344,24 @@
     </row>
     <row r="47">
       <c r="A47" s="4" t="n"/>
-      <c r="B47" s="4" t="n"/>
-      <c r="C47" s="4" t="n"/>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t>Nike</t>
+        </is>
+      </c>
+      <c r="C47" s="4" t="inlineStr">
+        <is>
+          <t>Zoom Fly</t>
+        </is>
+      </c>
       <c r="D47" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E47" t="n">
-        <v>11111119</v>
+        <v>11111129</v>
       </c>
       <c r="F47" t="n">
-        <v>2000000</v>
+        <v>2500000</v>
       </c>
       <c r="G47" t="n">
         <v>10</v>
@@ -1371,21 +1369,13 @@
     </row>
     <row r="48">
       <c r="A48" s="4" t="n"/>
-      <c r="B48" s="4" t="inlineStr">
-        <is>
-          <t>Nike</t>
-        </is>
-      </c>
-      <c r="C48" s="4" t="inlineStr">
-        <is>
-          <t>Zoom Fly</t>
-        </is>
-      </c>
+      <c r="B48" s="4" t="n"/>
+      <c r="C48" s="4" t="n"/>
       <c r="D48" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E48" t="n">
-        <v>11111129</v>
+        <v>11111130</v>
       </c>
       <c r="F48" t="n">
         <v>2500000</v>
@@ -1399,10 +1389,10 @@
       <c r="B49" s="4" t="n"/>
       <c r="C49" s="4" t="n"/>
       <c r="D49" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E49" t="n">
-        <v>11111130</v>
+        <v>11111131</v>
       </c>
       <c r="F49" t="n">
         <v>2500000</v>
@@ -1416,10 +1406,10 @@
       <c r="B50" s="4" t="n"/>
       <c r="C50" s="4" t="n"/>
       <c r="D50" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E50" t="n">
-        <v>11111131</v>
+        <v>11111132</v>
       </c>
       <c r="F50" t="n">
         <v>2500000</v>
@@ -1433,10 +1423,10 @@
       <c r="B51" s="4" t="n"/>
       <c r="C51" s="4" t="n"/>
       <c r="D51" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E51" t="n">
-        <v>11111132</v>
+        <v>11111133</v>
       </c>
       <c r="F51" t="n">
         <v>2500000</v>
@@ -1450,10 +1440,10 @@
       <c r="B52" s="4" t="n"/>
       <c r="C52" s="4" t="n"/>
       <c r="D52" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E52" t="n">
-        <v>11111133</v>
+        <v>11111134</v>
       </c>
       <c r="F52" t="n">
         <v>2500000</v>
@@ -1467,10 +1457,10 @@
       <c r="B53" s="4" t="n"/>
       <c r="C53" s="4" t="n"/>
       <c r="D53" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E53" t="n">
-        <v>11111134</v>
+        <v>11111135</v>
       </c>
       <c r="F53" t="n">
         <v>2500000</v>
@@ -1484,10 +1474,10 @@
       <c r="B54" s="4" t="n"/>
       <c r="C54" s="4" t="n"/>
       <c r="D54" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E54" t="n">
-        <v>11111135</v>
+        <v>11111136</v>
       </c>
       <c r="F54" t="n">
         <v>2500000</v>
@@ -1501,56 +1491,56 @@
       <c r="B55" s="4" t="n"/>
       <c r="C55" s="4" t="n"/>
       <c r="D55" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E55" t="n">
-        <v>11111136</v>
+        <v>11111137</v>
       </c>
       <c r="F55" t="n">
         <v>2500000</v>
       </c>
       <c r="G55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="n"/>
-      <c r="B56" s="4" t="n"/>
-      <c r="C56" s="4" t="n"/>
+      <c r="A56" s="4" t="inlineStr">
+        <is>
+          <t>Sneaker</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adidas </t>
+        </is>
+      </c>
+      <c r="C56" s="4" t="inlineStr">
+        <is>
+          <t>Samba</t>
+        </is>
+      </c>
       <c r="D56" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E56" t="n">
-        <v>11111137</v>
+        <v>11111174</v>
       </c>
       <c r="F56" t="n">
-        <v>2500000</v>
+        <v>1750000</v>
       </c>
       <c r="G56" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="4" t="inlineStr">
-        <is>
-          <t>Sneaker</t>
-        </is>
-      </c>
-      <c r="B57" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C57" s="4" t="inlineStr">
-        <is>
-          <t>Samba</t>
-        </is>
-      </c>
+      <c r="A57" s="4" t="n"/>
+      <c r="B57" s="4" t="n"/>
+      <c r="C57" s="4" t="n"/>
       <c r="D57" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E57" t="n">
-        <v>11111174</v>
+        <v>11111175</v>
       </c>
       <c r="F57" t="n">
         <v>1750000</v>
@@ -1564,10 +1554,10 @@
       <c r="B58" s="4" t="n"/>
       <c r="C58" s="4" t="n"/>
       <c r="D58" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E58" t="n">
-        <v>11111175</v>
+        <v>11111176</v>
       </c>
       <c r="F58" t="n">
         <v>1750000</v>
@@ -1581,10 +1571,10 @@
       <c r="B59" s="4" t="n"/>
       <c r="C59" s="4" t="n"/>
       <c r="D59" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E59" t="n">
-        <v>11111176</v>
+        <v>11111177</v>
       </c>
       <c r="F59" t="n">
         <v>1750000</v>
@@ -1598,10 +1588,10 @@
       <c r="B60" s="4" t="n"/>
       <c r="C60" s="4" t="n"/>
       <c r="D60" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E60" t="n">
-        <v>11111177</v>
+        <v>11111178</v>
       </c>
       <c r="F60" t="n">
         <v>1750000</v>
@@ -1615,10 +1605,10 @@
       <c r="B61" s="4" t="n"/>
       <c r="C61" s="4" t="n"/>
       <c r="D61" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E61" t="n">
-        <v>11111178</v>
+        <v>11111179</v>
       </c>
       <c r="F61" t="n">
         <v>1750000</v>
@@ -1632,10 +1622,10 @@
       <c r="B62" s="4" t="n"/>
       <c r="C62" s="4" t="n"/>
       <c r="D62" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E62" t="n">
-        <v>11111179</v>
+        <v>11111180</v>
       </c>
       <c r="F62" t="n">
         <v>1750000</v>
@@ -1649,10 +1639,10 @@
       <c r="B63" s="4" t="n"/>
       <c r="C63" s="4" t="n"/>
       <c r="D63" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E63" t="n">
-        <v>11111180</v>
+        <v>11111181</v>
       </c>
       <c r="F63" t="n">
         <v>1750000</v>
@@ -1666,10 +1656,10 @@
       <c r="B64" s="4" t="n"/>
       <c r="C64" s="4" t="n"/>
       <c r="D64" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E64" t="n">
-        <v>11111181</v>
+        <v>11111182</v>
       </c>
       <c r="F64" t="n">
         <v>1750000</v>
@@ -1681,15 +1671,19 @@
     <row r="65">
       <c r="A65" s="4" t="n"/>
       <c r="B65" s="4" t="n"/>
-      <c r="C65" s="4" t="n"/>
+      <c r="C65" s="4" t="inlineStr">
+        <is>
+          <t>Yeezy</t>
+        </is>
+      </c>
       <c r="D65" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E65" t="n">
-        <v>11111182</v>
+        <v>11111165</v>
       </c>
       <c r="F65" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G65" t="n">
         <v>10</v>
@@ -1698,16 +1692,12 @@
     <row r="66">
       <c r="A66" s="4" t="n"/>
       <c r="B66" s="4" t="n"/>
-      <c r="C66" s="4" t="inlineStr">
-        <is>
-          <t>Yeezy</t>
-        </is>
-      </c>
+      <c r="C66" s="4" t="n"/>
       <c r="D66" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E66" t="n">
-        <v>11111165</v>
+        <v>11111166</v>
       </c>
       <c r="F66" t="n">
         <v>3500000</v>
@@ -1721,10 +1711,10 @@
       <c r="B67" s="4" t="n"/>
       <c r="C67" s="4" t="n"/>
       <c r="D67" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E67" t="n">
-        <v>11111166</v>
+        <v>11111167</v>
       </c>
       <c r="F67" t="n">
         <v>3500000</v>
@@ -1738,10 +1728,10 @@
       <c r="B68" s="4" t="n"/>
       <c r="C68" s="4" t="n"/>
       <c r="D68" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E68" t="n">
-        <v>11111167</v>
+        <v>11111168</v>
       </c>
       <c r="F68" t="n">
         <v>3500000</v>
@@ -1755,10 +1745,10 @@
       <c r="B69" s="4" t="n"/>
       <c r="C69" s="4" t="n"/>
       <c r="D69" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E69" t="n">
-        <v>11111168</v>
+        <v>11111169</v>
       </c>
       <c r="F69" t="n">
         <v>3500000</v>
@@ -1772,10 +1762,10 @@
       <c r="B70" s="4" t="n"/>
       <c r="C70" s="4" t="n"/>
       <c r="D70" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E70" t="n">
-        <v>11111169</v>
+        <v>11111170</v>
       </c>
       <c r="F70" t="n">
         <v>3500000</v>
@@ -1789,10 +1779,10 @@
       <c r="B71" s="4" t="n"/>
       <c r="C71" s="4" t="n"/>
       <c r="D71" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E71" t="n">
-        <v>11111170</v>
+        <v>11111171</v>
       </c>
       <c r="F71" t="n">
         <v>3500000</v>
@@ -1806,10 +1796,10 @@
       <c r="B72" s="4" t="n"/>
       <c r="C72" s="4" t="n"/>
       <c r="D72" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E72" t="n">
-        <v>11111171</v>
+        <v>11111172</v>
       </c>
       <c r="F72" t="n">
         <v>3500000</v>
@@ -1823,10 +1813,10 @@
       <c r="B73" s="4" t="n"/>
       <c r="C73" s="4" t="n"/>
       <c r="D73" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E73" t="n">
-        <v>11111172</v>
+        <v>11111173</v>
       </c>
       <c r="F73" t="n">
         <v>3500000</v>
@@ -1837,16 +1827,22 @@
     </row>
     <row r="74">
       <c r="A74" s="4" t="n"/>
-      <c r="B74" s="4" t="n"/>
-      <c r="C74" s="4" t="n"/>
+      <c r="B74" s="4" t="inlineStr">
+        <is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C74" s="4" t="n">
+        <v>550</v>
+      </c>
       <c r="D74" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E74" t="n">
-        <v>11111173</v>
+        <v>11111147</v>
       </c>
       <c r="F74" t="n">
-        <v>3500000</v>
+        <v>2500000</v>
       </c>
       <c r="G74" t="n">
         <v>10</v>
@@ -1854,19 +1850,13 @@
     </row>
     <row r="75">
       <c r="A75" s="4" t="n"/>
-      <c r="B75" s="4" t="inlineStr">
-        <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C75" s="4" t="n">
-        <v>550</v>
-      </c>
+      <c r="B75" s="4" t="n"/>
+      <c r="C75" s="4" t="n"/>
       <c r="D75" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E75" t="n">
-        <v>11111147</v>
+        <v>11111148</v>
       </c>
       <c r="F75" t="n">
         <v>2500000</v>
@@ -1880,10 +1870,10 @@
       <c r="B76" s="4" t="n"/>
       <c r="C76" s="4" t="n"/>
       <c r="D76" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E76" t="n">
-        <v>11111148</v>
+        <v>11111149</v>
       </c>
       <c r="F76" t="n">
         <v>2500000</v>
@@ -1897,10 +1887,10 @@
       <c r="B77" s="4" t="n"/>
       <c r="C77" s="4" t="n"/>
       <c r="D77" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E77" t="n">
-        <v>11111149</v>
+        <v>11111150</v>
       </c>
       <c r="F77" t="n">
         <v>2500000</v>
@@ -1914,10 +1904,10 @@
       <c r="B78" s="4" t="n"/>
       <c r="C78" s="4" t="n"/>
       <c r="D78" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E78" t="n">
-        <v>11111150</v>
+        <v>11111151</v>
       </c>
       <c r="F78" t="n">
         <v>2500000</v>
@@ -1931,10 +1921,10 @@
       <c r="B79" s="4" t="n"/>
       <c r="C79" s="4" t="n"/>
       <c r="D79" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E79" t="n">
-        <v>11111151</v>
+        <v>11111152</v>
       </c>
       <c r="F79" t="n">
         <v>2500000</v>
@@ -1948,10 +1938,10 @@
       <c r="B80" s="4" t="n"/>
       <c r="C80" s="4" t="n"/>
       <c r="D80" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E80" t="n">
-        <v>11111152</v>
+        <v>11111153</v>
       </c>
       <c r="F80" t="n">
         <v>2500000</v>
@@ -1965,10 +1955,10 @@
       <c r="B81" s="4" t="n"/>
       <c r="C81" s="4" t="n"/>
       <c r="D81" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E81" t="n">
-        <v>11111153</v>
+        <v>11111154</v>
       </c>
       <c r="F81" t="n">
         <v>2500000</v>
@@ -1982,10 +1972,10 @@
       <c r="B82" s="4" t="n"/>
       <c r="C82" s="4" t="n"/>
       <c r="D82" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E82" t="n">
-        <v>11111154</v>
+        <v>11111155</v>
       </c>
       <c r="F82" t="n">
         <v>2500000</v>
@@ -1996,16 +1986,24 @@
     </row>
     <row r="83">
       <c r="A83" s="4" t="n"/>
-      <c r="B83" s="4" t="n"/>
-      <c r="C83" s="4" t="n"/>
+      <c r="B83" s="4" t="inlineStr">
+        <is>
+          <t>Nike</t>
+        </is>
+      </c>
+      <c r="C83" s="4" t="inlineStr">
+        <is>
+          <t>Air Force 1</t>
+        </is>
+      </c>
       <c r="D83" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E83" t="n">
-        <v>11111155</v>
+        <v>11111156</v>
       </c>
       <c r="F83" t="n">
-        <v>2500000</v>
+        <v>1500000</v>
       </c>
       <c r="G83" t="n">
         <v>10</v>
@@ -2013,21 +2011,13 @@
     </row>
     <row r="84">
       <c r="A84" s="4" t="n"/>
-      <c r="B84" s="4" t="inlineStr">
-        <is>
-          <t>Nike</t>
-        </is>
-      </c>
-      <c r="C84" s="4" t="inlineStr">
-        <is>
-          <t>Air Force 1</t>
-        </is>
-      </c>
+      <c r="B84" s="4" t="n"/>
+      <c r="C84" s="4" t="n"/>
       <c r="D84" s="4" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E84" t="n">
-        <v>11111156</v>
+        <v>11111157</v>
       </c>
       <c r="F84" t="n">
         <v>1500000</v>
@@ -2041,10 +2031,10 @@
       <c r="B85" s="4" t="n"/>
       <c r="C85" s="4" t="n"/>
       <c r="D85" s="4" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E85" t="n">
-        <v>11111157</v>
+        <v>11111158</v>
       </c>
       <c r="F85" t="n">
         <v>1500000</v>
@@ -2058,10 +2048,10 @@
       <c r="B86" s="4" t="n"/>
       <c r="C86" s="4" t="n"/>
       <c r="D86" s="4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E86" t="n">
-        <v>11111158</v>
+        <v>11111159</v>
       </c>
       <c r="F86" t="n">
         <v>1500000</v>
@@ -2075,10 +2065,10 @@
       <c r="B87" s="4" t="n"/>
       <c r="C87" s="4" t="n"/>
       <c r="D87" s="4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E87" t="n">
-        <v>11111159</v>
+        <v>11111160</v>
       </c>
       <c r="F87" t="n">
         <v>1500000</v>
@@ -2092,10 +2082,10 @@
       <c r="B88" s="4" t="n"/>
       <c r="C88" s="4" t="n"/>
       <c r="D88" s="4" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E88" t="n">
-        <v>11111160</v>
+        <v>11111161</v>
       </c>
       <c r="F88" t="n">
         <v>1500000</v>
@@ -2109,10 +2099,10 @@
       <c r="B89" s="4" t="n"/>
       <c r="C89" s="4" t="n"/>
       <c r="D89" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E89" t="n">
-        <v>11111161</v>
+        <v>11111162</v>
       </c>
       <c r="F89" t="n">
         <v>1500000</v>
@@ -2126,10 +2116,10 @@
       <c r="B90" s="4" t="n"/>
       <c r="C90" s="4" t="n"/>
       <c r="D90" s="4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E90" t="n">
-        <v>11111162</v>
+        <v>11111163</v>
       </c>
       <c r="F90" t="n">
         <v>1500000</v>
@@ -2143,10 +2133,10 @@
       <c r="B91" s="4" t="n"/>
       <c r="C91" s="4" t="n"/>
       <c r="D91" s="4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E91" t="n">
-        <v>11111163</v>
+        <v>11111164</v>
       </c>
       <c r="F91" t="n">
         <v>1500000</v>
@@ -2155,47 +2145,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="4" t="n"/>
-      <c r="B92" s="4" t="n"/>
-      <c r="C92" s="4" t="n"/>
-      <c r="D92" s="4" t="n">
-        <v>45</v>
-      </c>
-      <c r="E92" t="n">
-        <v>11111164</v>
-      </c>
-      <c r="F92" t="n">
-        <v>1500000</v>
-      </c>
-      <c r="G92" t="n">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C84:C92"/>
-    <mergeCell ref="A21:A56"/>
-    <mergeCell ref="B57:B74"/>
-    <mergeCell ref="B39:B47"/>
-    <mergeCell ref="A57:A92"/>
-    <mergeCell ref="C75:C83"/>
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="C12:C20"/>
-    <mergeCell ref="C21:C29"/>
-    <mergeCell ref="B48:B56"/>
-    <mergeCell ref="B84:B92"/>
-    <mergeCell ref="C39:C47"/>
-    <mergeCell ref="C57:C65"/>
-    <mergeCell ref="C48:C56"/>
-    <mergeCell ref="C66:C74"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="C3:C11"/>
-    <mergeCell ref="B75:B83"/>
-    <mergeCell ref="C30:C38"/>
-    <mergeCell ref="B12:B20"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="C65:C73"/>
+    <mergeCell ref="C47:C55"/>
+    <mergeCell ref="C56:C64"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="B29:B37"/>
+    <mergeCell ref="B38:B46"/>
+    <mergeCell ref="C11:C19"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="A20:A55"/>
+    <mergeCell ref="B83:B91"/>
+    <mergeCell ref="B74:B82"/>
+    <mergeCell ref="C38:C46"/>
+    <mergeCell ref="B20:B28"/>
+    <mergeCell ref="C74:C82"/>
+    <mergeCell ref="C83:C91"/>
+    <mergeCell ref="B56:B73"/>
+    <mergeCell ref="B47:B55"/>
+    <mergeCell ref="C20:C28"/>
+    <mergeCell ref="C29:C37"/>
+    <mergeCell ref="B11:B19"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="A56:A91"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix = main menu gapake class
</commit_message>
<xml_diff>
--- a/Persediaan1.xlsx
+++ b/Persediaan1.xlsx
@@ -1500,7 +1500,7 @@
         <v>2500000</v>
       </c>
       <c r="G55" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56">
@@ -2142,7 +2142,7 @@
         <v>1500000</v>
       </c>
       <c r="G91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix = main menu fix
</commit_message>
<xml_diff>
--- a/Persediaan1.xlsx
+++ b/Persediaan1.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1549,7 +1549,7 @@
         <v>3000000</v>
       </c>
       <c r="G37" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -1576,7 +1576,7 @@
         <v>2500000</v>
       </c>
       <c r="G38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -2575,7 +2575,7 @@
         <v>1750000</v>
       </c>
       <c r="G73" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74">
@@ -3098,70 +3098,6 @@
       </c>
       <c r="G91" t="n">
         <v>10</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>Elektronik</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Samsung</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>A54</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>101010</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>Transportasi</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Toyota</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Camry</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>202020</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix : benerin program
</commit_message>
<xml_diff>
--- a/Persediaan1.xlsx
+++ b/Persediaan1.xlsx
@@ -2,28 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Persediaan1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -37,12 +41,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -55,16 +74,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -147,44 +173,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -211,14 +237,32 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -245,6 +289,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -256,166 +318,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -425,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,37 +472,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>jenis</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>merek</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>series</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>ukuran</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>kode</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>harga</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>jumlah</t>
         </is>
@@ -473,56 +511,56 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hoka </t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Arahi 7</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>37</v>
       </c>
       <c r="E2" t="n">
-        <v>11111111</v>
+        <v>11111183</v>
       </c>
       <c r="F2" t="n">
-        <v>2000000</v>
+        <v>750000</v>
       </c>
       <c r="G2" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hoka </t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Arahi 7</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D3" t="n">
         <v>38</v>
       </c>
       <c r="E3" t="n">
-        <v>11111112</v>
+        <v>11111184</v>
       </c>
       <c r="F3" t="n">
-        <v>2000000</v>
+        <v>750000</v>
       </c>
       <c r="G3" t="n">
         <v>10</v>
@@ -531,27 +569,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hoka </t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Arahi 7</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>39</v>
       </c>
       <c r="E4" t="n">
-        <v>11111113</v>
+        <v>11111185</v>
       </c>
       <c r="F4" t="n">
-        <v>2000000</v>
+        <v>750000</v>
       </c>
       <c r="G4" t="n">
         <v>10</v>
@@ -560,27 +598,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hoka </t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Arahi 7</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>40</v>
       </c>
       <c r="E5" t="n">
-        <v>11111114</v>
+        <v>11111186</v>
       </c>
       <c r="F5" t="n">
-        <v>2000000</v>
+        <v>750000</v>
       </c>
       <c r="G5" t="n">
         <v>10</v>
@@ -589,27 +627,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hoka </t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Arahi 7</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>41</v>
       </c>
       <c r="E6" t="n">
-        <v>11111115</v>
+        <v>11111187</v>
       </c>
       <c r="F6" t="n">
-        <v>2000000</v>
+        <v>750000</v>
       </c>
       <c r="G6" t="n">
         <v>10</v>
@@ -618,27 +656,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hoka </t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Arahi 7</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D7" t="n">
         <v>42</v>
       </c>
       <c r="E7" t="n">
-        <v>11111116</v>
+        <v>11111188</v>
       </c>
       <c r="F7" t="n">
-        <v>2000000</v>
+        <v>750000</v>
       </c>
       <c r="G7" t="n">
         <v>10</v>
@@ -647,27 +685,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hoka </t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Arahi 7</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D8" t="n">
         <v>43</v>
       </c>
       <c r="E8" t="n">
-        <v>11111117</v>
+        <v>11111189</v>
       </c>
       <c r="F8" t="n">
-        <v>2000000</v>
+        <v>750000</v>
       </c>
       <c r="G8" t="n">
         <v>10</v>
@@ -676,27 +714,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hoka </t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Arahi 7</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D9" t="n">
         <v>44</v>
       </c>
       <c r="E9" t="n">
-        <v>11111118</v>
+        <v>11111190</v>
       </c>
       <c r="F9" t="n">
-        <v>2000000</v>
+        <v>750000</v>
       </c>
       <c r="G9" t="n">
         <v>10</v>
@@ -705,27 +743,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hoka </t>
+          <t xml:space="preserve">Adidas </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Arahi 7</t>
+          <t>Adilette</t>
         </is>
       </c>
       <c r="D10" t="n">
         <v>45</v>
       </c>
       <c r="E10" t="n">
-        <v>11111119</v>
+        <v>11111191</v>
       </c>
       <c r="F10" t="n">
-        <v>2000000</v>
+        <v>750000</v>
       </c>
       <c r="G10" t="n">
         <v>10</v>
@@ -734,27 +772,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Asics</t>
+          <t xml:space="preserve">Nike </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Gel-Nimbus</t>
+          <t xml:space="preserve">Benassi </t>
         </is>
       </c>
       <c r="D11" t="n">
         <v>37</v>
       </c>
       <c r="E11" t="n">
-        <v>11111120</v>
+        <v>11111192</v>
       </c>
       <c r="F11" t="n">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="G11" t="n">
         <v>10</v>
@@ -763,27 +801,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Asics</t>
+          <t xml:space="preserve">Nike </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Gel-Nimbus</t>
+          <t xml:space="preserve">Benassi </t>
         </is>
       </c>
       <c r="D12" t="n">
         <v>38</v>
       </c>
       <c r="E12" t="n">
-        <v>11111121</v>
+        <v>11111193</v>
       </c>
       <c r="F12" t="n">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="G12" t="n">
         <v>10</v>
@@ -792,27 +830,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Asics</t>
+          <t xml:space="preserve">Nike </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gel-Nimbus</t>
+          <t xml:space="preserve">Benassi </t>
         </is>
       </c>
       <c r="D13" t="n">
         <v>39</v>
       </c>
       <c r="E13" t="n">
-        <v>11111122</v>
+        <v>11111194</v>
       </c>
       <c r="F13" t="n">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="G13" t="n">
         <v>10</v>
@@ -821,27 +859,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Asics</t>
+          <t xml:space="preserve">Nike </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Gel-Nimbus</t>
+          <t xml:space="preserve">Benassi </t>
         </is>
       </c>
       <c r="D14" t="n">
         <v>40</v>
       </c>
       <c r="E14" t="n">
-        <v>11111123</v>
+        <v>11111195</v>
       </c>
       <c r="F14" t="n">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="G14" t="n">
         <v>10</v>
@@ -850,27 +888,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Asics</t>
+          <t xml:space="preserve">Nike </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Gel-Nimbus</t>
+          <t xml:space="preserve">Benassi </t>
         </is>
       </c>
       <c r="D15" t="n">
         <v>41</v>
       </c>
       <c r="E15" t="n">
-        <v>11111124</v>
+        <v>11111196</v>
       </c>
       <c r="F15" t="n">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="G15" t="n">
         <v>10</v>
@@ -879,27 +917,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Asics</t>
+          <t xml:space="preserve">Nike </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Gel-Nimbus</t>
+          <t xml:space="preserve">Benassi </t>
         </is>
       </c>
       <c r="D16" t="n">
         <v>42</v>
       </c>
       <c r="E16" t="n">
-        <v>11111125</v>
+        <v>11111197</v>
       </c>
       <c r="F16" t="n">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="G16" t="n">
         <v>10</v>
@@ -908,27 +946,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Asics</t>
+          <t xml:space="preserve">Nike </t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Gel-Nimbus</t>
+          <t xml:space="preserve">Benassi </t>
         </is>
       </c>
       <c r="D17" t="n">
         <v>43</v>
       </c>
       <c r="E17" t="n">
-        <v>11111126</v>
+        <v>11111198</v>
       </c>
       <c r="F17" t="n">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="G17" t="n">
         <v>10</v>
@@ -937,27 +975,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Asics</t>
+          <t xml:space="preserve">Nike </t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Gel-Nimbus</t>
+          <t xml:space="preserve">Benassi </t>
         </is>
       </c>
       <c r="D18" t="n">
         <v>44</v>
       </c>
       <c r="E18" t="n">
-        <v>11111127</v>
+        <v>11111199</v>
       </c>
       <c r="F18" t="n">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="G18" t="n">
         <v>10</v>
@@ -966,27 +1004,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Running</t>
+          <t>Flip Flops</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Asics</t>
+          <t xml:space="preserve">Nike </t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Gel-Nimbus</t>
+          <t xml:space="preserve">Benassi </t>
         </is>
       </c>
       <c r="D19" t="n">
         <v>45</v>
       </c>
       <c r="E19" t="n">
-        <v>11111128</v>
+        <v>11111200</v>
       </c>
       <c r="F19" t="n">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="G19" t="n">
         <v>10</v>
@@ -1000,25 +1038,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Nike</t>
+          <t>Adidas</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Zoom Fly</t>
+          <t>Adizero</t>
         </is>
       </c>
       <c r="D20" t="n">
         <v>37</v>
       </c>
       <c r="E20" t="n">
-        <v>11111129</v>
+        <v>11111138</v>
       </c>
       <c r="F20" t="n">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -1029,22 +1067,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Nike</t>
+          <t>Adidas</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Zoom Fly</t>
+          <t>Adizero</t>
         </is>
       </c>
       <c r="D21" t="n">
         <v>38</v>
       </c>
       <c r="E21" t="n">
-        <v>11111130</v>
+        <v>11111139</v>
       </c>
       <c r="F21" t="n">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G21" t="n">
         <v>10</v>
@@ -1058,22 +1096,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nike</t>
+          <t>Adidas</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Zoom Fly</t>
+          <t>Adizero</t>
         </is>
       </c>
       <c r="D22" t="n">
         <v>39</v>
       </c>
       <c r="E22" t="n">
-        <v>11111131</v>
+        <v>11111140</v>
       </c>
       <c r="F22" t="n">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G22" t="n">
         <v>10</v>
@@ -1087,22 +1125,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Nike</t>
+          <t>Adidas</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Zoom Fly</t>
+          <t>Adizero</t>
         </is>
       </c>
       <c r="D23" t="n">
         <v>40</v>
       </c>
       <c r="E23" t="n">
-        <v>11111132</v>
+        <v>11111141</v>
       </c>
       <c r="F23" t="n">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G23" t="n">
         <v>10</v>
@@ -1116,22 +1154,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Nike</t>
+          <t>Adidas</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Zoom Fly</t>
+          <t>Adizero</t>
         </is>
       </c>
       <c r="D24" t="n">
         <v>41</v>
       </c>
       <c r="E24" t="n">
-        <v>11111133</v>
+        <v>11111142</v>
       </c>
       <c r="F24" t="n">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G24" t="n">
         <v>10</v>
@@ -1145,22 +1183,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Nike</t>
+          <t>Adidas</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Zoom Fly</t>
+          <t>Adizero</t>
         </is>
       </c>
       <c r="D25" t="n">
         <v>42</v>
       </c>
       <c r="E25" t="n">
-        <v>11111134</v>
+        <v>11111143</v>
       </c>
       <c r="F25" t="n">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G25" t="n">
         <v>10</v>
@@ -1174,22 +1212,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Nike</t>
+          <t>Adidas</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Zoom Fly</t>
+          <t>Adizero</t>
         </is>
       </c>
       <c r="D26" t="n">
         <v>43</v>
       </c>
       <c r="E26" t="n">
-        <v>11111135</v>
+        <v>11111144</v>
       </c>
       <c r="F26" t="n">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G26" t="n">
         <v>10</v>
@@ -1203,22 +1241,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Nike</t>
+          <t>Adidas</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Zoom Fly</t>
+          <t>Adizero</t>
         </is>
       </c>
       <c r="D27" t="n">
         <v>44</v>
       </c>
       <c r="E27" t="n">
-        <v>11111136</v>
+        <v>11111145</v>
       </c>
       <c r="F27" t="n">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G27" t="n">
         <v>10</v>
@@ -1232,22 +1270,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Nike</t>
+          <t>Adidas</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Zoom Fly</t>
+          <t>Adizero</t>
         </is>
       </c>
       <c r="D28" t="n">
         <v>45</v>
       </c>
       <c r="E28" t="n">
-        <v>11111137</v>
+        <v>11111146</v>
       </c>
       <c r="F28" t="n">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G28" t="n">
         <v>10</v>
@@ -1261,22 +1299,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Adidas</t>
+          <t>Asics</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Adizero</t>
+          <t>Gel-Nimbus</t>
         </is>
       </c>
       <c r="D29" t="n">
         <v>37</v>
       </c>
       <c r="E29" t="n">
-        <v>11111138</v>
+        <v>11111120</v>
       </c>
       <c r="F29" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G29" t="n">
         <v>10</v>
@@ -1290,22 +1328,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Adidas</t>
+          <t>Asics</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Adizero</t>
+          <t>Gel-Nimbus</t>
         </is>
       </c>
       <c r="D30" t="n">
         <v>38</v>
       </c>
       <c r="E30" t="n">
-        <v>11111139</v>
+        <v>11111121</v>
       </c>
       <c r="F30" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G30" t="n">
         <v>10</v>
@@ -1319,22 +1357,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Adidas</t>
+          <t>Asics</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Adizero</t>
+          <t>Gel-Nimbus</t>
         </is>
       </c>
       <c r="D31" t="n">
         <v>39</v>
       </c>
       <c r="E31" t="n">
-        <v>11111140</v>
+        <v>11111122</v>
       </c>
       <c r="F31" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G31" t="n">
         <v>10</v>
@@ -1348,22 +1386,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Adidas</t>
+          <t>Asics</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Adizero</t>
+          <t>Gel-Nimbus</t>
         </is>
       </c>
       <c r="D32" t="n">
         <v>40</v>
       </c>
       <c r="E32" t="n">
-        <v>11111141</v>
+        <v>11111123</v>
       </c>
       <c r="F32" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G32" t="n">
         <v>10</v>
@@ -1377,22 +1415,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Adidas</t>
+          <t>Asics</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Adizero</t>
+          <t>Gel-Nimbus</t>
         </is>
       </c>
       <c r="D33" t="n">
         <v>41</v>
       </c>
       <c r="E33" t="n">
-        <v>11111142</v>
+        <v>11111124</v>
       </c>
       <c r="F33" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G33" t="n">
         <v>10</v>
@@ -1406,22 +1444,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Adidas</t>
+          <t>Asics</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Adizero</t>
+          <t>Gel-Nimbus</t>
         </is>
       </c>
       <c r="D34" t="n">
         <v>42</v>
       </c>
       <c r="E34" t="n">
-        <v>11111143</v>
+        <v>11111125</v>
       </c>
       <c r="F34" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G34" t="n">
         <v>10</v>
@@ -1435,22 +1473,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Adidas</t>
+          <t>Asics</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Adizero</t>
+          <t>Gel-Nimbus</t>
         </is>
       </c>
       <c r="D35" t="n">
         <v>43</v>
       </c>
       <c r="E35" t="n">
-        <v>11111144</v>
+        <v>11111126</v>
       </c>
       <c r="F35" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G35" t="n">
         <v>10</v>
@@ -1464,22 +1502,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Adidas</t>
+          <t>Asics</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Adizero</t>
+          <t>Gel-Nimbus</t>
         </is>
       </c>
       <c r="D36" t="n">
         <v>44</v>
       </c>
       <c r="E36" t="n">
-        <v>11111145</v>
+        <v>11111127</v>
       </c>
       <c r="F36" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G36" t="n">
         <v>10</v>
@@ -1493,22 +1531,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Adidas</t>
+          <t>Asics</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Adizero</t>
+          <t>Gel-Nimbus</t>
         </is>
       </c>
       <c r="D37" t="n">
         <v>45</v>
       </c>
       <c r="E37" t="n">
-        <v>11111146</v>
+        <v>11111128</v>
       </c>
       <c r="F37" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
       <c r="G37" t="n">
         <v>10</v>
@@ -1517,52 +1555,56 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
-        <v>550</v>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
       </c>
       <c r="D38" t="n">
         <v>37</v>
       </c>
       <c r="E38" t="n">
-        <v>11111147</v>
+        <v>11111111</v>
       </c>
       <c r="F38" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="G38" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C39" t="n">
-        <v>550</v>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
       </c>
       <c r="D39" t="n">
         <v>38</v>
       </c>
       <c r="E39" t="n">
-        <v>11111148</v>
+        <v>11111112</v>
       </c>
       <c r="F39" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="G39" t="n">
         <v>10</v>
@@ -1571,25 +1613,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
-        <v>550</v>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
       </c>
       <c r="D40" t="n">
         <v>39</v>
       </c>
       <c r="E40" t="n">
-        <v>11111149</v>
+        <v>11111113</v>
       </c>
       <c r="F40" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="G40" t="n">
         <v>10</v>
@@ -1598,25 +1642,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C41" t="n">
-        <v>550</v>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
       </c>
       <c r="D41" t="n">
         <v>40</v>
       </c>
       <c r="E41" t="n">
-        <v>11111150</v>
+        <v>11111114</v>
       </c>
       <c r="F41" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="G41" t="n">
         <v>10</v>
@@ -1625,25 +1671,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>550</v>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
       </c>
       <c r="D42" t="n">
         <v>41</v>
       </c>
       <c r="E42" t="n">
-        <v>11111151</v>
+        <v>11111115</v>
       </c>
       <c r="F42" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="G42" t="n">
         <v>10</v>
@@ -1652,25 +1700,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
-        <v>550</v>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
       </c>
       <c r="D43" t="n">
         <v>42</v>
       </c>
       <c r="E43" t="n">
-        <v>11111152</v>
+        <v>11111116</v>
       </c>
       <c r="F43" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="G43" t="n">
         <v>10</v>
@@ -1679,25 +1729,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
-        <v>550</v>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
       </c>
       <c r="D44" t="n">
         <v>43</v>
       </c>
       <c r="E44" t="n">
-        <v>11111153</v>
+        <v>11111117</v>
       </c>
       <c r="F44" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="G44" t="n">
         <v>10</v>
@@ -1706,25 +1758,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
-        <v>550</v>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
       </c>
       <c r="D45" t="n">
         <v>44</v>
       </c>
       <c r="E45" t="n">
-        <v>11111154</v>
+        <v>11111118</v>
       </c>
       <c r="F45" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="G45" t="n">
         <v>10</v>
@@ -1733,25 +1787,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>New Balance</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>550</v>
+          <t xml:space="preserve">Hoka </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Arahi 7</t>
+        </is>
       </c>
       <c r="D46" t="n">
         <v>45</v>
       </c>
       <c r="E46" t="n">
-        <v>11111155</v>
+        <v>11111119</v>
       </c>
       <c r="F46" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="G46" t="n">
         <v>10</v>
@@ -1760,7 +1816,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1770,17 +1826,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Air Force 1</t>
+          <t>Zoom Fly</t>
         </is>
       </c>
       <c r="D47" t="n">
         <v>37</v>
       </c>
       <c r="E47" t="n">
-        <v>11111156</v>
+        <v>11111129</v>
       </c>
       <c r="F47" t="n">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="G47" t="n">
         <v>10</v>
@@ -1789,7 +1845,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1799,17 +1855,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Air Force 1</t>
+          <t>Zoom Fly</t>
         </is>
       </c>
       <c r="D48" t="n">
         <v>38</v>
       </c>
       <c r="E48" t="n">
-        <v>11111157</v>
+        <v>11111130</v>
       </c>
       <c r="F48" t="n">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="G48" t="n">
         <v>10</v>
@@ -1818,7 +1874,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1828,17 +1884,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Air Force 1</t>
+          <t>Zoom Fly</t>
         </is>
       </c>
       <c r="D49" t="n">
         <v>39</v>
       </c>
       <c r="E49" t="n">
-        <v>11111158</v>
+        <v>11111131</v>
       </c>
       <c r="F49" t="n">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="G49" t="n">
         <v>10</v>
@@ -1847,7 +1903,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1857,17 +1913,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Air Force 1</t>
+          <t>Zoom Fly</t>
         </is>
       </c>
       <c r="D50" t="n">
         <v>40</v>
       </c>
       <c r="E50" t="n">
-        <v>11111159</v>
+        <v>11111132</v>
       </c>
       <c r="F50" t="n">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="G50" t="n">
         <v>10</v>
@@ -1876,7 +1932,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1886,17 +1942,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Air Force 1</t>
+          <t>Zoom Fly</t>
         </is>
       </c>
       <c r="D51" t="n">
         <v>41</v>
       </c>
       <c r="E51" t="n">
-        <v>11111160</v>
+        <v>11111133</v>
       </c>
       <c r="F51" t="n">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="G51" t="n">
         <v>10</v>
@@ -1905,7 +1961,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1915,17 +1971,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Air Force 1</t>
+          <t>Zoom Fly</t>
         </is>
       </c>
       <c r="D52" t="n">
         <v>42</v>
       </c>
       <c r="E52" t="n">
-        <v>11111161</v>
+        <v>11111134</v>
       </c>
       <c r="F52" t="n">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="G52" t="n">
         <v>10</v>
@@ -1934,7 +1990,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1944,17 +2000,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Air Force 1</t>
+          <t>Zoom Fly</t>
         </is>
       </c>
       <c r="D53" t="n">
         <v>43</v>
       </c>
       <c r="E53" t="n">
-        <v>11111162</v>
+        <v>11111135</v>
       </c>
       <c r="F53" t="n">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="G53" t="n">
         <v>10</v>
@@ -1963,7 +2019,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1973,17 +2029,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Air Force 1</t>
+          <t>Zoom Fly</t>
         </is>
       </c>
       <c r="D54" t="n">
         <v>44</v>
       </c>
       <c r="E54" t="n">
-        <v>11111163</v>
+        <v>11111136</v>
       </c>
       <c r="F54" t="n">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="G54" t="n">
         <v>10</v>
@@ -1992,7 +2048,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Sneaker</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2002,17 +2058,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Air Force 1</t>
+          <t>Zoom Fly</t>
         </is>
       </c>
       <c r="D55" t="n">
         <v>45</v>
       </c>
       <c r="E55" t="n">
-        <v>11111164</v>
+        <v>11111137</v>
       </c>
       <c r="F55" t="n">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="G55" t="n">
         <v>10</v>
@@ -2031,17 +2087,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Yeezy</t>
+          <t>Samba</t>
         </is>
       </c>
       <c r="D56" t="n">
         <v>37</v>
       </c>
       <c r="E56" t="n">
-        <v>11111165</v>
+        <v>11111174</v>
       </c>
       <c r="F56" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="G56" t="n">
         <v>10</v>
@@ -2060,17 +2116,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Yeezy</t>
+          <t>Samba</t>
         </is>
       </c>
       <c r="D57" t="n">
         <v>38</v>
       </c>
       <c r="E57" t="n">
-        <v>11111166</v>
+        <v>11111175</v>
       </c>
       <c r="F57" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="G57" t="n">
         <v>10</v>
@@ -2089,17 +2145,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Yeezy</t>
+          <t>Samba</t>
         </is>
       </c>
       <c r="D58" t="n">
         <v>39</v>
       </c>
       <c r="E58" t="n">
-        <v>11111167</v>
+        <v>11111176</v>
       </c>
       <c r="F58" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="G58" t="n">
         <v>10</v>
@@ -2118,17 +2174,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Yeezy</t>
+          <t>Samba</t>
         </is>
       </c>
       <c r="D59" t="n">
         <v>40</v>
       </c>
       <c r="E59" t="n">
-        <v>11111168</v>
+        <v>11111177</v>
       </c>
       <c r="F59" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="G59" t="n">
         <v>10</v>
@@ -2147,17 +2203,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Yeezy</t>
+          <t>Samba</t>
         </is>
       </c>
       <c r="D60" t="n">
         <v>41</v>
       </c>
       <c r="E60" t="n">
-        <v>11111169</v>
+        <v>11111178</v>
       </c>
       <c r="F60" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="G60" t="n">
         <v>10</v>
@@ -2176,17 +2232,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Yeezy</t>
+          <t>Samba</t>
         </is>
       </c>
       <c r="D61" t="n">
         <v>42</v>
       </c>
       <c r="E61" t="n">
-        <v>11111170</v>
+        <v>11111179</v>
       </c>
       <c r="F61" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="G61" t="n">
         <v>10</v>
@@ -2205,17 +2261,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Yeezy</t>
+          <t>Samba</t>
         </is>
       </c>
       <c r="D62" t="n">
         <v>43</v>
       </c>
       <c r="E62" t="n">
-        <v>11111171</v>
+        <v>11111180</v>
       </c>
       <c r="F62" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="G62" t="n">
         <v>10</v>
@@ -2234,17 +2290,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Yeezy</t>
+          <t>Samba</t>
         </is>
       </c>
       <c r="D63" t="n">
         <v>44</v>
       </c>
       <c r="E63" t="n">
-        <v>11111172</v>
+        <v>11111181</v>
       </c>
       <c r="F63" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="G63" t="n">
         <v>10</v>
@@ -2263,17 +2319,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Yeezy</t>
+          <t>Samba</t>
         </is>
       </c>
       <c r="D64" t="n">
         <v>45</v>
       </c>
       <c r="E64" t="n">
-        <v>11111173</v>
+        <v>11111182</v>
       </c>
       <c r="F64" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="G64" t="n">
         <v>10</v>
@@ -2292,17 +2348,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Samba</t>
+          <t>Yeezy</t>
         </is>
       </c>
       <c r="D65" t="n">
         <v>37</v>
       </c>
       <c r="E65" t="n">
-        <v>11111174</v>
+        <v>11111165</v>
       </c>
       <c r="F65" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G65" t="n">
         <v>10</v>
@@ -2321,17 +2377,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Samba</t>
+          <t>Yeezy</t>
         </is>
       </c>
       <c r="D66" t="n">
         <v>38</v>
       </c>
       <c r="E66" t="n">
-        <v>11111175</v>
+        <v>11111166</v>
       </c>
       <c r="F66" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G66" t="n">
         <v>10</v>
@@ -2350,17 +2406,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Samba</t>
+          <t>Yeezy</t>
         </is>
       </c>
       <c r="D67" t="n">
         <v>39</v>
       </c>
       <c r="E67" t="n">
-        <v>11111176</v>
+        <v>11111167</v>
       </c>
       <c r="F67" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G67" t="n">
         <v>10</v>
@@ -2379,17 +2435,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Samba</t>
+          <t>Yeezy</t>
         </is>
       </c>
       <c r="D68" t="n">
         <v>40</v>
       </c>
       <c r="E68" t="n">
-        <v>11111177</v>
+        <v>11111168</v>
       </c>
       <c r="F68" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G68" t="n">
         <v>10</v>
@@ -2408,17 +2464,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Samba</t>
+          <t>Yeezy</t>
         </is>
       </c>
       <c r="D69" t="n">
         <v>41</v>
       </c>
       <c r="E69" t="n">
-        <v>11111178</v>
+        <v>11111169</v>
       </c>
       <c r="F69" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G69" t="n">
         <v>10</v>
@@ -2437,17 +2493,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Samba</t>
+          <t>Yeezy</t>
         </is>
       </c>
       <c r="D70" t="n">
         <v>42</v>
       </c>
       <c r="E70" t="n">
-        <v>11111179</v>
+        <v>11111170</v>
       </c>
       <c r="F70" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G70" t="n">
         <v>10</v>
@@ -2466,17 +2522,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Samba</t>
+          <t>Yeezy</t>
         </is>
       </c>
       <c r="D71" t="n">
         <v>43</v>
       </c>
       <c r="E71" t="n">
-        <v>11111180</v>
+        <v>11111171</v>
       </c>
       <c r="F71" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G71" t="n">
         <v>10</v>
@@ -2495,17 +2551,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Samba</t>
+          <t>Yeezy</t>
         </is>
       </c>
       <c r="D72" t="n">
         <v>44</v>
       </c>
       <c r="E72" t="n">
-        <v>11111181</v>
+        <v>11111172</v>
       </c>
       <c r="F72" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G72" t="n">
         <v>10</v>
@@ -2524,17 +2580,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Samba</t>
+          <t>Yeezy</t>
         </is>
       </c>
       <c r="D73" t="n">
         <v>45</v>
       </c>
       <c r="E73" t="n">
-        <v>11111182</v>
+        <v>11111173</v>
       </c>
       <c r="F73" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="G73" t="n">
         <v>10</v>
@@ -2543,27 +2599,25 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>550</v>
       </c>
       <c r="D74" t="n">
         <v>37</v>
       </c>
       <c r="E74" t="n">
-        <v>11111183</v>
+        <v>11111147</v>
       </c>
       <c r="F74" t="n">
-        <v>750000</v>
+        <v>2500000</v>
       </c>
       <c r="G74" t="n">
         <v>10</v>
@@ -2572,27 +2626,25 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>550</v>
       </c>
       <c r="D75" t="n">
         <v>38</v>
       </c>
       <c r="E75" t="n">
-        <v>11111184</v>
+        <v>11111148</v>
       </c>
       <c r="F75" t="n">
-        <v>750000</v>
+        <v>2500000</v>
       </c>
       <c r="G75" t="n">
         <v>10</v>
@@ -2601,27 +2653,25 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>550</v>
       </c>
       <c r="D76" t="n">
         <v>39</v>
       </c>
       <c r="E76" t="n">
-        <v>11111185</v>
+        <v>11111149</v>
       </c>
       <c r="F76" t="n">
-        <v>750000</v>
+        <v>2500000</v>
       </c>
       <c r="G76" t="n">
         <v>10</v>
@@ -2630,27 +2680,25 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>550</v>
       </c>
       <c r="D77" t="n">
         <v>40</v>
       </c>
       <c r="E77" t="n">
-        <v>11111186</v>
+        <v>11111150</v>
       </c>
       <c r="F77" t="n">
-        <v>750000</v>
+        <v>2500000</v>
       </c>
       <c r="G77" t="n">
         <v>10</v>
@@ -2659,27 +2707,25 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>550</v>
       </c>
       <c r="D78" t="n">
         <v>41</v>
       </c>
       <c r="E78" t="n">
-        <v>11111187</v>
+        <v>11111151</v>
       </c>
       <c r="F78" t="n">
-        <v>750000</v>
+        <v>2500000</v>
       </c>
       <c r="G78" t="n">
         <v>10</v>
@@ -2688,27 +2734,25 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>550</v>
       </c>
       <c r="D79" t="n">
         <v>42</v>
       </c>
       <c r="E79" t="n">
-        <v>11111188</v>
+        <v>11111152</v>
       </c>
       <c r="F79" t="n">
-        <v>750000</v>
+        <v>2500000</v>
       </c>
       <c r="G79" t="n">
         <v>10</v>
@@ -2717,27 +2761,25 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>550</v>
       </c>
       <c r="D80" t="n">
         <v>43</v>
       </c>
       <c r="E80" t="n">
-        <v>11111189</v>
+        <v>11111153</v>
       </c>
       <c r="F80" t="n">
-        <v>750000</v>
+        <v>2500000</v>
       </c>
       <c r="G80" t="n">
         <v>10</v>
@@ -2746,27 +2788,25 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>550</v>
       </c>
       <c r="D81" t="n">
         <v>44</v>
       </c>
       <c r="E81" t="n">
-        <v>11111190</v>
+        <v>11111154</v>
       </c>
       <c r="F81" t="n">
-        <v>750000</v>
+        <v>2500000</v>
       </c>
       <c r="G81" t="n">
         <v>10</v>
@@ -2775,27 +2815,25 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adidas </t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Adilette</t>
-        </is>
+          <t>New Balance</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>550</v>
       </c>
       <c r="D82" t="n">
         <v>45</v>
       </c>
       <c r="E82" t="n">
-        <v>11111191</v>
+        <v>11111155</v>
       </c>
       <c r="F82" t="n">
-        <v>750000</v>
+        <v>2500000</v>
       </c>
       <c r="G82" t="n">
         <v>10</v>
@@ -2804,27 +2842,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nike </t>
+          <t>Nike</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benassi </t>
+          <t>Air Force 1</t>
         </is>
       </c>
       <c r="D83" t="n">
         <v>37</v>
       </c>
       <c r="E83" t="n">
-        <v>11111192</v>
+        <v>11111156</v>
       </c>
       <c r="F83" t="n">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="G83" t="n">
         <v>10</v>
@@ -2833,27 +2871,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nike </t>
+          <t>Nike</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benassi </t>
+          <t>Air Force 1</t>
         </is>
       </c>
       <c r="D84" t="n">
         <v>38</v>
       </c>
       <c r="E84" t="n">
-        <v>11111193</v>
+        <v>11111157</v>
       </c>
       <c r="F84" t="n">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="G84" t="n">
         <v>10</v>
@@ -2862,27 +2900,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nike </t>
+          <t>Nike</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benassi </t>
+          <t>Air Force 1</t>
         </is>
       </c>
       <c r="D85" t="n">
         <v>39</v>
       </c>
       <c r="E85" t="n">
-        <v>11111194</v>
+        <v>11111158</v>
       </c>
       <c r="F85" t="n">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="G85" t="n">
         <v>10</v>
@@ -2891,27 +2929,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nike </t>
+          <t>Nike</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benassi </t>
+          <t>Air Force 1</t>
         </is>
       </c>
       <c r="D86" t="n">
         <v>40</v>
       </c>
       <c r="E86" t="n">
-        <v>11111195</v>
+        <v>11111159</v>
       </c>
       <c r="F86" t="n">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="G86" t="n">
         <v>10</v>
@@ -2920,27 +2958,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nike </t>
+          <t>Nike</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benassi </t>
+          <t>Air Force 1</t>
         </is>
       </c>
       <c r="D87" t="n">
         <v>41</v>
       </c>
       <c r="E87" t="n">
-        <v>11111196</v>
+        <v>11111160</v>
       </c>
       <c r="F87" t="n">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="G87" t="n">
         <v>10</v>
@@ -2949,27 +2987,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nike </t>
+          <t>Nike</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benassi </t>
+          <t>Air Force 1</t>
         </is>
       </c>
       <c r="D88" t="n">
         <v>42</v>
       </c>
       <c r="E88" t="n">
-        <v>11111197</v>
+        <v>11111161</v>
       </c>
       <c r="F88" t="n">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="G88" t="n">
         <v>10</v>
@@ -2978,27 +3016,27 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nike </t>
+          <t>Nike</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benassi </t>
+          <t>Air Force 1</t>
         </is>
       </c>
       <c r="D89" t="n">
         <v>43</v>
       </c>
       <c r="E89" t="n">
-        <v>11111198</v>
+        <v>11111162</v>
       </c>
       <c r="F89" t="n">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="G89" t="n">
         <v>10</v>
@@ -3007,27 +3045,27 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nike </t>
+          <t>Nike</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benassi </t>
+          <t>Air Force 1</t>
         </is>
       </c>
       <c r="D90" t="n">
         <v>44</v>
       </c>
       <c r="E90" t="n">
-        <v>11111199</v>
+        <v>11111163</v>
       </c>
       <c r="F90" t="n">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="G90" t="n">
         <v>10</v>
@@ -3036,27 +3074,27 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Flip Flops</t>
+          <t>Sneaker</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nike </t>
+          <t>Nike</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benassi </t>
+          <t>Air Force 1</t>
         </is>
       </c>
       <c r="D91" t="n">
         <v>45</v>
       </c>
       <c r="E91" t="n">
-        <v>11111200</v>
+        <v>11111164</v>
       </c>
       <c r="F91" t="n">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="G91" t="n">
         <v>10</v>
@@ -3065,117 +3103,30 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Elektronik</t>
+          <t>yam</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>nyam</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>A54</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="E92" t="n">
-        <v>101010</v>
+        <v>41243062</v>
       </c>
       <c r="F92" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>Transportasi</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Toyota</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Camry</t>
-        </is>
-      </c>
-      <c r="D93" t="n">
-        <v>4</v>
-      </c>
-      <c r="E93" t="n">
-        <v>202020</v>
-      </c>
-      <c r="F93" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>Transportasi</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Boeing</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>737</t>
-        </is>
-      </c>
-      <c r="D94" t="n">
-        <v>700</v>
-      </c>
-      <c r="E94" t="n">
-        <v>36496422</v>
-      </c>
-      <c r="F94" t="n">
-        <v>626262</v>
-      </c>
-      <c r="G94" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>ghu</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>h8iik</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>koo</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
-      </c>
-      <c r="E95" t="n">
-        <v>17410175</v>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>876678</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+        <v>1000</v>
+      </c>
+      <c r="G92" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>